<commit_message>
Refactor BMW scraping script to use logging
Replaced print statements with Python's logging module for improved output control and clarity. Refactored car data extraction into a function, added error handling, and updated summary and export steps to use logging. Limited car processing to first 10 links for testing and improved equipment extraction logic.
</commit_message>
<xml_diff>
--- a/results/bmw/bmw_cars_2025-11-01.xlsx
+++ b/results/bmw/bmw_cars_2025-11-01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -617,6 +617,879 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BMW i4 eDrive40 Gran Coupé</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>21284</v>
+      </c>
+      <c r="C3" t="n">
+        <v>58900</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>58 900,00 €</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>250</v>
+      </c>
+      <c r="J3" t="n">
+        <v>340</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>250 kW (340 PS)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>{
+  "Charging": [
+    "Adaptateur pour prise domestique (type E+F)",
+    "Câble de recharge rapide jusqu'à 22kW (Mode 3)",
+    "Flexible Fast Charger (mode 2)"
+  ],
+  "Equipements électriques": [
+    "Adaptive LED headlights",
+    "BMW IconicSounds Electric",
+    "Climatisation à réglage électronique",
+    "Driving Assistant Pack Professional",
+    "High Beam Assist",
+    "M Lights Shadow Line",
+    "Parking Assistant Pack Plus",
+    "Système d'alarme"
+  ],
+  "Equipements extérieurs": [
+    "Accès confort",
+    "Spoiler arrière M",
+    "Kit aérodynamique M",
+    "M Shadow Line hochglänzend",
+    "M Shadow Line hochglänzend avec éléments supplémentaires",
+    "Vitres teintées foncées à l'arrière"
+  ],
+  "Equipements intérieurs": [
+    "Ceintures de sécurité M",
+    "Lumière intérieure d'ambiance",
+    "Ciel de pavillon M en Anthrazit",
+    "Pack rangement",
+    "Pack rétroviseurs",
+    "Réglage en largeur du dossier pour conducteur",
+    "Rétroviseur intérieur anti-éblouissement automatique",
+    "Sièges chauffants à l'avant",
+    "Soutien lombaire à l'avant",
+    "Volant M sport"
+  ],
+  "Télécommunication embarquée": [
+    "BMW Live Cockpit Navigation Professional avec Head-Up Display",
+    "Espace de rangement pour Wireless Charging",
+    "Harman/kardon Surround Sound System",
+    "Intelligent Emergency Call - eCall",
+    "Personal eSIM"
+  ],
+  "Transmission, suspension et direction": [
+    "Attelage de remorque (rabattable électriquement)",
+    "Freins M Sport, rot",
+    "Volant M sport"
+  ],
+  "Autres.": [
+    "Code interne",
+    "Code interne",
+    "Code interne",
+    "Code interne"
+  ]
+}</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0194dfaa-ef28-7c5f-86fa-47075dd521df?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0475&amp;fabric=FVATQ&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05YA,S05DN,S06NX,S07M9,S08WC,S03AC,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S06VB,S033B,S0302,S03M2,S0548,S05DA,S07LG,S0420,S0491,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AU,S04GQ,S02PA,S04LN,S08TR,S0688,S03FK,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BMW i4 eDrive35 Gran Coupé M Edition</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>14074</v>
+      </c>
+      <c r="C4" t="n">
+        <v>58500</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>58 500,00 €</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>15001</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>15001 km</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-05-01</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>mai 2025</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>210</v>
+      </c>
+      <c r="J4" t="n">
+        <v>286</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>210 kW (286 PS)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>{
+  "Charging": [
+    "Câble de recharge rapide jusqu'à 22kW (Mode 3)"
+  ],
+  "Equipements électriques": [
+    "Climatisation à réglage électronique",
+    "Driving Assistant Pack Professional",
+    "Parking Assistant Pack Plus",
+    "Système d'alarme"
+  ],
+  "Equipements extérieurs": [
+    "Étriers de frein, laqués (blau)",
+    "Accès confort",
+    "Kit aérodynamique M",
+    "M Shadow Line hochglänzend",
+    "Vitres teintées foncées à l'arrière"
+  ],
+  "Equipements intérieurs": [
+    "Lumière intérieure d'ambiance",
+    "Ciel de pavillon M en Anthrazit",
+    "Pack rangement",
+    "Pack rétroviseurs",
+    "Rétroviseur intérieur anti-éblouissement automatique",
+    "Sièges chauffants à l'avant",
+    "Soutien lombaire à l'avant",
+    "Toit ouvrant à commande électrique",
+    "Volant chauffant",
+    "Volant M sport"
+  ],
+  "Télécommunication embarquée": [
+    "BMW Live Cockpit Navigation Professional avec Head-Up Display",
+    "Espace de rangement pour Wireless Charging",
+    "Intelligent Emergency Call - eCall",
+    "Personal eSIM",
+    "Système haut-parleurs HiFi"
+  ],
+  "Transmission, suspension et direction": [
+    "Étriers de frein, laqués (blau)",
+    "Attelage de remorque (rabattable électriquement)",
+    "Volant M sport"
+  ],
+  "Autres.": [
+    "Code interne",
+    "Code interne",
+    "Code interne",
+    "Code interne"
+  ]
+}</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01939440-204d-7b22-a0d1-1d4ed0ed596f?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=1EHD&amp;paint=P0C36&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05DN,S06NX,S02BQ,S08WC,S03AC,S0775,S0676,S0710,S0534,S0337,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S06PA,S05AU,S06VB,S02PA,S0302,S04LN,S08TR,S0248,S0403,S0548,S03FA,S0760,S05DA,S07LG,S0420,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BMW i4 xDrive40 Gran Coupé</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>14070</v>
+      </c>
+      <c r="C5" t="n">
+        <v>55900</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>55 900,00 €</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>295</v>
+      </c>
+      <c r="J5" t="n">
+        <v>401</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>295 kW (401 PS)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>{
+  "Charging": [
+    "Câble de recharge rapide jusqu'à 22kW (Mode 3)"
+  ],
+  "Equipements électriques": [
+    "Adaptive LED headlights",
+    "Climatisation à réglage électronique",
+    "Driving Assistant Pack Professional",
+    "High Beam Assist",
+    "M Lights Shadow Line",
+    "Parking Assistant Pack Plus",
+    "Système d'alarme"
+  ],
+  "Equipements extérieurs": [
+    "Spoiler arrière M",
+    "Kit aérodynamique M",
+    "M Shadow Line hochglänzend",
+    "M Shadow Line hochglänzend avec éléments supplémentaires",
+    "Vitres teintées foncées à l'arrière"
+  ],
+  "Equipements intérieurs": [
+    "Ceintures de sécurité M",
+    "Lumière intérieure d'ambiance",
+    "Ciel de pavillon M en Anthrazit",
+    "Pack rangement",
+    "Pack rétroviseurs",
+    "Réglage électrique des sièges avant, avec fonction-mémoire pour siège conducteur",
+    "Rétroviseur intérieur anti-éblouissement automatique",
+    "Sièges chauffants à l'avant",
+    "Volant chauffant",
+    "Volant M sport"
+  ],
+  "Télécommunication embarquée": [
+    "BMW Live Cockpit Navigation Professional avec Head-Up Display",
+    "Harman/kardon Surround Sound System",
+    "Intelligent Emergency Call - eCall",
+    "Personal eSIM"
+  ],
+  "Transmission, suspension et direction": [
+    "Attelage de remorque (rabattable électriquement)",
+    "Freins M Sport, rot",
+    "Suspension adaptative M",
+    "Variable Sport Steering",
+    "Volant M sport"
+  ],
+  "Autres.": [
+    "Code interne",
+    "Code interne",
+    "Code interne"
+  ]
+}</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0194fadf-2025-7a82-80aa-adc54fe8ab1e?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41HD&amp;paint=P0C4P&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S07M9,S03AC,S0775,S0710,S0754,S0534,S0337,S05AC,S0459,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S0552,S06PA,S02VL,S05AU,S04GQ,S06VB,S033B,S02VF,S02PA,S0302,S04LN,S08TR,S0688,S0248,S03M2,S0548,S03FA,S0760,S05DA,S0420,S06U3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BMW i4 eDrive40 Gran Coupé</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>44976</v>
+      </c>
+      <c r="C6" t="n">
+        <v>55900</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>55 900,00 €</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>250</v>
+      </c>
+      <c r="J6" t="n">
+        <v>340</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>250 kW (340 PS)</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>{
+  "Charging": [
+    "Adaptateur pour prise domestique (type E+F)",
+    "Câble de recharge rapide jusqu'à 22kW (Mode 3)",
+    "Flexible Fast Charger (mode 2)"
+  ],
+  "Equipements électriques": [
+    "Adaptive LED headlights",
+    "BMW IconicSounds Electric",
+    "Climatisation à réglage électronique",
+    "Cruise Control",
+    "Driving Assistant Pack",
+    "High Beam Assist",
+    "Parking Assistant Pack Plus",
+    "Système d'alarme"
+  ],
+  "Equipements extérieurs": [
+    "Étriers de frein, laqués (blau)",
+    "Accès confort",
+    "Kit aérodynamique M",
+    "M Shadow Line hochglänzend",
+    "Vitres teintées foncées à l'arrière"
+  ],
+  "Equipements intérieurs": [
+    "Lumière intérieure d'ambiance",
+    "Ciel de pavillon M en Anthrazit",
+    "Pack rangement",
+    "Pack rétroviseurs",
+    "Réglage en largeur du dossier pour conducteur",
+    "Rétroviseur intérieur anti-éblouissement automatique",
+    "Sièges chauffants à l'avant",
+    "Soutien lombaire à l'avant",
+    "Toit ouvrant à commande électrique",
+    "Volant M sport"
+  ],
+  "Télécommunication embarquée": [
+    "BMW Live Cockpit Navigation Professional avec Head-Up Display",
+    "Espace de rangement pour Wireless Charging",
+    "Harman/kardon Surround Sound System",
+    "Intelligent Emergency Call - eCall",
+    "Personal eSIM"
+  ],
+  "Transmission, suspension et direction": [
+    "Étriers de frein, laqués (blau)",
+    "Attelage de remorque (rabattable électriquement)",
+    "Volant M sport"
+  ],
+  "Autres.": [
+    "Code interne",
+    "Code interne",
+    "Code interne",
+    "Code interne"
+  ]
+}</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0194b79a-6463-7a38-8ef9-60a42d15a197?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0300&amp;fabric=FMANL&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05YA,S05DN,S06NX,S02BQ,S08WC,S03AC,S0710,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S06VB,S0302,S0544,S0548,S05DA,S07LG,S0420,S03FX,S04MC,S0491,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AS,S09QY,S02PA,S0688,S0403,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>BMW i4 eDrive40 Gran Coupé</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>27917</v>
+      </c>
+      <c r="C7" t="n">
+        <v>54900</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>54 900,00 €</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>250</v>
+      </c>
+      <c r="J7" t="n">
+        <v>340</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>250 kW (340 PS)</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>{
+  "Charging": [
+    "Adaptateur pour prise domestique (type E+F)",
+    "Câble de recharge rapide jusqu'à 22kW (Mode 3)",
+    "Flexible Fast Charger (mode 2)"
+  ],
+  "Equipements électriques": [
+    "Adaptive LED headlights",
+    "BMW IconicSounds Electric",
+    "Climatisation à réglage électronique",
+    "Driving Assistant Pack Professional",
+    "High Beam Assist",
+    "M Lights Shadow Line",
+    "Parking Assistant Pack Plus",
+    "Système d'alarme"
+  ],
+  "Equipements extérieurs": [
+    "Accès confort",
+    "Spoiler arrière M",
+    "Kit aérodynamique M",
+    "M Shadow Line hochglänzend",
+    "M Shadow Line hochglänzend avec éléments supplémentaires",
+    "Vitres teintées foncées à l'arrière"
+  ],
+  "Equipements intérieurs": [
+    "Ceintures de sécurité M",
+    "Lumière intérieure d'ambiance",
+    "Ciel de pavillon M en Anthrazit",
+    "Pack rangement",
+    "Pack rétroviseurs",
+    "Réglage en largeur du dossier pour conducteur",
+    "Rétroviseur intérieur anti-éblouissement automatique",
+    "Sièges chauffants à l'avant",
+    "Soutien lombaire à l'avant",
+    "Volant chauffant",
+    "Volant M sport"
+  ],
+  "Télécommunication embarquée": [
+    "BMW Live Cockpit Navigation Professional avec Head-Up Display",
+    "Espace de rangement pour Wireless Charging",
+    "Intelligent Emergency Call - eCall",
+    "Personal eSIM",
+    "Système haut-parleurs HiFi"
+  ],
+  "Transmission, suspension et direction": [
+    "Attelage de remorque (rabattable électriquement)",
+    "Freins M Sport, rot",
+    "Volant M sport"
+  ],
+  "Autres.": [
+    "Code interne",
+    "Code interne",
+    "Code interne",
+    "Code interne"
+  ]
+}</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0194ac16-7276-7b16-9471-4874d13d68d6?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C3Z&amp;fabric=FEPMI&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05YA,S05DN,S06NX,S07M9,S08WC,S03AC,S0676,S0710,S0754,S05AC,S0715,S04H0,S08WN,S0430,S0431,S04T2,S0552,S04T3,S06VB,S033B,S03GX,S0302,S03M2,S0548,S05DA,S07LG,S0420,S0491,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AU,S04GQ,S02PA,S08TR,S0248,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>BMW i4 eDrive40 Gran Coupé</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1295</v>
+      </c>
+      <c r="C8" t="n">
+        <v>57900</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>57 900,00 €</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>250</v>
+      </c>
+      <c r="J8" t="n">
+        <v>340</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>250 kW (340 PS)</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>{
+  "Charging": [
+    "Câble de recharge rapide jusqu'à 22kW (Mode 3)"
+  ],
+  "Equipements électriques": [
+    "Active Cruise Control avec fonction Stop&amp;Go",
+    "Adaptive LED headlights",
+    "Climatisation à réglage électronique",
+    "High Beam Assist",
+    "M Lights Shadow Line",
+    "Parking Assistant Pack",
+    "Système d'alarme"
+  ],
+  "Equipements extérieurs": [
+    "Accès confort",
+    "Spoiler arrière M",
+    "Kit aérodynamique M",
+    "M Shadow Line hochglänzend",
+    "M Shadow Line hochglänzend avec éléments supplémentaires",
+    "Vitres teintées foncées à l'arrière"
+  ],
+  "Equipements intérieurs": [
+    "Ceintures de sécurité M",
+    "Lumière intérieure d'ambiance",
+    "Ciel de pavillon M en Anthrazit",
+    "Pack rangement",
+    "Pack rétroviseurs",
+    "Réglage électrique des sièges avant, avec fonction-mémoire pour siège conducteur",
+    "Rétroviseur intérieur anti-éblouissement automatique",
+    "Sièges chauffants à l'avant",
+    "Soutien lombaire à l'avant",
+    "Volant M sport"
+  ],
+  "Télécommunication embarquée": [
+    "BMW Live Cockpit Navigation Plus",
+    "Espace de rangement pour Wireless Charging",
+    "Intelligent Emergency Call - eCall",
+    "Personal eSIM"
+  ],
+  "Transmission, suspension et direction": [
+    "Freins M Sport, rot",
+    "Volant M sport"
+  ],
+  "Autres.": [
+    "Code interne",
+    "Code interne",
+    "Code interne",
+    "Code interne"
+  ]
+}</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01943b89-5a88-7ce1-9a07-575165faba41?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0475&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S08WD,S03MF,S05DM,S06NX,S06WC,S07M9,S08WC,S0775,S0710,S0754,S0534,S0337,S05AC,S0459,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S0552,S06PA,S04H1,S04GQ,S06VB,S033B,S02PA,S0302,S05DF,S03FK,S03M2,S0548,S0760,S05DA,S07LG,S0420,S06U2,S0322,S0488</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>BMW i4 xDrive40 Gran Coupé</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>44651</v>
+      </c>
+      <c r="C9" t="n">
+        <v>56750</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>56 750,00 €</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>295</v>
+      </c>
+      <c r="J9" t="n">
+        <v>401</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>295 kW (401 PS)</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>{
+  "Charging": [
+    "Adaptateur pour prise domestique (type E+F)",
+    "Câble de recharge rapide jusqu'à 22kW (Mode 3)",
+    "Flexible Fast Charger (mode 2)"
+  ],
+  "Equipements électriques": [
+    "Adaptive LED headlights",
+    "BMW IconicSounds Electric",
+    "Climatisation à réglage électronique",
+    "Driving Assistant Pack Professional",
+    "High Beam Assist",
+    "Parking Assistant Pack Plus",
+    "Système d'alarme"
+  ],
+  "Equipements extérieurs": [
+    "Étriers de frein, laqués (blau)",
+    "Accès confort",
+    "Kit aérodynamique M",
+    "M Shadow Line hochglänzend",
+    "Vitres teintées foncées à l'arrière"
+  ],
+  "Equipements intérieurs": [
+    "Lumière intérieure d'ambiance",
+    "Ciel de pavillon M en Anthrazit",
+    "Pack rangement",
+    "Pack rétroviseurs",
+    "Réglage électrique des sièges avant, avec fonction-mémoire pour siège conducteur",
+    "Rétroviseur intérieur anti-éblouissement automatique",
+    "Sièges chauffants à l'avant",
+    "Soutien lombaire à l'avant",
+    "Volant chauffant",
+    "Volant M sport"
+  ],
+  "Télécommunication embarquée": [
+    "BMW Live Cockpit Navigation Professional avec Head-Up Display",
+    "Espace de rangement pour Wireless Charging",
+    "Intelligent Emergency Call - eCall",
+    "Personal eSIM",
+    "Système haut-parleurs HiFi"
+  ],
+  "Transmission, suspension et direction": [
+    "Étriers de frein, laqués (blau)",
+    "Suspension adaptative M",
+    "Variable Sport Steering",
+    "Volant M sport"
+  ],
+  "Autres.": [
+    "Code interne",
+    "Code interne",
+    "Code interne",
+    "Code interne"
+  ]
+}</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01928951-520f-7327-9e7d-1db572a24367?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41HD&amp;paint=P0C5Y&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05YA,S05DN,S06NX,S02BQ,S0676,S0710,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S02VL,S06VB,S02VF,S0302,S0548,S05DA,S07LG,S0420,S03FX,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AU,S02PA,S04LN,S08TR,S0248,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>BMW i4 xDrive40 Gran Coupé</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>44516</v>
+      </c>
+      <c r="C10" t="n">
+        <v>56900</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>56 900,00 €</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>295</v>
+      </c>
+      <c r="J10" t="n">
+        <v>401</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>295 kW (401 PS)</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>{
+  "Charging": [
+    "Adaptateur pour prise domestique (type E+F)",
+    "Câble de recharge rapide jusqu'à 22kW (Mode 3)",
+    "Flexible Fast Charger (mode 2)"
+  ],
+  "Equipements électriques": [
+    "Adaptive LED headlights",
+    "BMW IconicSounds Electric",
+    "Climatisation à réglage électronique",
+    "Driving Assistant Pack Professional",
+    "High Beam Assist",
+    "Parking Assistant Pack Plus",
+    "Système d'alarme"
+  ],
+  "Equipements extérieurs": [
+    "Étriers de frein, laqués (blau)",
+    "Accès confort",
+    "Kit aérodynamique M",
+    "M Shadow Line hochglänzend",
+    "Vitres teintées foncées à l'arrière"
+  ],
+  "Equipements intérieurs": [
+    "Eléments intérieur avec finition en cristal 'CraftedClarity'",
+    "Lumière intérieure d'ambiance",
+    "Ciel de pavillon M en Anthrazit",
+    "Pack rangement",
+    "Pack rétroviseurs",
+    "Réglage en largeur du dossier pour conducteur",
+    "Réglage électrique des sièges avant, avec fonction-mémoire pour siège conducteur",
+    "Rétroviseur intérieur anti-éblouissement automatique",
+    "Sièges chauffants à l'avant et à l'arrière",
+    "Soutien lombaire à l'avant",
+    "Toit ouvrant à commande électrique",
+    "Volant chauffant",
+    "Volant M sport"
+  ],
+  "Télécommunication embarquée": [
+    "BMW Live Cockpit Navigation Professional avec Head-Up Display",
+    "Espace de rangement pour Wireless Charging",
+    "Intelligent Emergency Call - eCall",
+    "Personal eSIM",
+    "Système haut-parleurs HiFi"
+  ],
+  "Transmission, suspension et direction": [
+    "Étriers de frein, laqués (blau)",
+    "Attelage de remorque (rabattable électriquement)",
+    "Suspension adaptative M",
+    "Variable Sport Steering",
+    "Volant M sport"
+  ],
+  "Autres.": [
+    "Code interne",
+    "Code interne",
+    "Code interne",
+    "Code interne"
+  ]
+}</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01927132-31bf-75f7-af77-3773e567d1e5?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41HD&amp;paint=P0C3Z&amp;fabric=FMAOI&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05YA,S05DN,S06NX,S02BQ,S03AC,S0676,S0710,S05AC,S0715,S04H0,S08WN,S0430,S0431,S04T2,S0552,S04T3,S02VL,S06VB,S02VF,S03GX,S0302,S0548,S05DA,S07LG,S0420,S04A2,S0491,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S04UR,S06PA,S05AU,S02PA,S08TR,S0248,S0403,S04HA,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BMW i4 eDrive40 Gran Coupé</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>38011</v>
+      </c>
+      <c r="C11" t="n">
+        <v>55490</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>55 490,00 €</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>250</v>
+      </c>
+      <c r="J11" t="n">
+        <v>340</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>250 kW (340 PS)</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>{
+  "Charging": [
+    "Adaptateur pour prise domestique (type E+F)",
+    "Câble de recharge rapide jusqu'à 22kW (Mode 3)",
+    "Flexible Fast Charger (mode 2)"
+  ],
+  "Equipements électriques": [
+    "Adaptive LED headlights",
+    "BMW IconicSounds Electric",
+    "Climatisation à réglage électronique",
+    "Cruise Control",
+    "Driving Assistant Pack",
+    "High Beam Assist",
+    "M Lights Shadow Line",
+    "Parking Assistant Pack Plus",
+    "Système d'alarme"
+  ],
+  "Equipements extérieurs": [
+    "Accès confort",
+    "Spoiler arrière M",
+    "Kit aérodynamique M",
+    "M Shadow Line hochglänzend",
+    "M Shadow Line hochglänzend avec éléments supplémentaires",
+    "Vitres teintées foncées à l'arrière"
+  ],
+  "Equipements intérieurs": [
+    "Ceintures de sécurité M",
+    "Lumière intérieure d'ambiance",
+    "Ciel de pavillon M en Anthrazit",
+    "Pack rangement",
+    "Pack rétroviseurs",
+    "Réglage en largeur du dossier pour conducteur",
+    "Rétroviseur intérieur anti-éblouissement automatique",
+    "Sièges chauffants à l'avant",
+    "Soutien lombaire à l'avant",
+    "Volant M sport"
+  ],
+  "Télécommunication embarquée": [
+    "BMW Live Cockpit Navigation Professional avec Head-Up Display",
+    "Espace de rangement pour Wireless Charging",
+    "Intelligent Emergency Call - eCall",
+    "Personal eSIM",
+    "Système haut-parleurs HiFi"
+  ],
+  "Transmission, suspension et direction": [
+    "Freins M Sport, rot",
+    "Volant M sport"
+  ],
+  "Autres.": [
+    "Code interne",
+    "Code interne",
+    "Code interne",
+    "Code interne"
+  ]
+}</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0192952f-08ab-7f33-aeb4-b2c696c84055?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C5Y&amp;fabric=FEPMI&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05YA,S05DN,S06NX,S07M9,S08WC,S0676,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S06VB,S033B,S0302,S0544,S03M2,S0548,S05DA,S07LG,S0420,S0491,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AS,S04H1,S04GQ,S09QY,S02PA,S03FA,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add historical tracking for BMW car inventory
Implemented historical tracking of BMW car inventory using SCD Type 2 logic in bmw_exploration.py. Added functions to load, merge, and export historical data to CSV, and updated the workflow to export only the latest records to Excel. Introduced results/bmw/bmw_cars_history.csv for storing historical records.
</commit_message>
<xml_diff>
--- a/results/bmw/bmw_cars_2025-11-01.xlsx
+++ b/results/bmw/bmw_cars_2025-11-01.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,14 +440,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>car_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>model_name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>car_id</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>price</t>
@@ -451,102 +455,95 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>price_raw</t>
+          <t>kilometers</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>kilometers</t>
+          <t>registration_date</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>kilometers_raw</t>
+          <t>horse_power_kw</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>registration_date</t>
+          <t>horse_power_ps</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>registration_date_raw</t>
+          <t>equipments</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>horse_power_kw</t>
+          <t>link</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>horse_power_ps</t>
+          <t>first_seen_date</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>horse_power_raw</t>
+          <t>last_seen_date</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>equipments</t>
+          <t>valid_from</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>valid_to</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>is_latest</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>scrape_date</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>39582</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>BMW i4 eDrive35 Gran Coupé M Edition</t>
         </is>
-      </c>
-      <c r="B2" t="n">
-        <v>39582</v>
       </c>
       <c r="C2" t="n">
         <v>59950</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>59 950,00 €</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+      <c r="D2" t="n">
         <v>9500</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>9500 km</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-08-01</t>
-        </is>
+      <c r="E2" s="2" t="n">
+        <v>45870</v>
+      </c>
+      <c r="F2" t="n">
+        <v>210</v>
+      </c>
+      <c r="G2" t="n">
+        <v>286</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>août 2025</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>210</v>
-      </c>
-      <c r="J2" t="n">
-        <v>286</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>210 kW (286 PS)</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -611,59 +608,70 @@
 }</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01966d0c-dbce-79bb-8cc6-ccd2613bd398?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=5EHD&amp;paint=P0C36&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S08WD,S03MF,S04NW,S05DM,S06NX,S06WC,S07M9,S08WC,S03AC,S0710,S0754,S05AC,S0715,S08WN,S0430,S08SM,S0431,S04T2,S0552,S02VL,S02VD,S06VB,S033B,S02VF,S0302,S05DF,S03M2,S0548,S05DA,S07LG,S0420,S04MC,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S0494,S04UR,S06PA,S05AS,S04GQ,S02PA,S0688,S0248,S0403,S03FK,S0760,S06U2,S0322,S0488</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01966d0c-dbce-79bb-8cc6-ccd2613bd398?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=5EHD&amp;paint=P0C36&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S08WD,S03MF,S04NW,S05DM,S06NX,S06WC,S07M9,S08WC,S03AC,S0710,S0754,S05AC,S0715,S08WN,S0430,S08SM,S0431,S04T2,S0552,S02VL,S02VD,S06VB,S033B,S02VF,S0302,S05DF,S03M2,S0548,S05DA,S07LG,S0420,S04MC,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S0494,S04UR,S06PA,S05AS,S04GQ,S02PA,S0688,S0248,S0403,S03FK,S0760,S06U2,S0322,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>14074</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>BMW i4 eDrive35 Gran Coupé M Edition</t>
         </is>
-      </c>
-      <c r="B3" t="n">
-        <v>14074</v>
       </c>
       <c r="C3" t="n">
         <v>58500</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>58 500,00 €</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
+      <c r="D3" t="n">
         <v>15001</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>15001 km</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-05-01</t>
-        </is>
+      <c r="E3" s="2" t="n">
+        <v>45778</v>
+      </c>
+      <c r="F3" t="n">
+        <v>210</v>
+      </c>
+      <c r="G3" t="n">
+        <v>286</v>
       </c>
       <c r="H3" t="inlineStr">
-        <is>
-          <t>mai 2025</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>210</v>
-      </c>
-      <c r="J3" t="n">
-        <v>286</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>210 kW (286 PS)</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -715,59 +723,70 @@
 }</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01939440-204d-7b22-a0d1-1d4ed0ed596f?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=1EHD&amp;paint=P0C36&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05DN,S06NX,S02BQ,S08WC,S03AC,S0775,S0676,S0710,S0534,S0337,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S06PA,S05AU,S06VB,S02PA,S0302,S04LN,S08TR,S0248,S0403,S0548,S03FA,S0760,S05DA,S07LG,S0420,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01939440-204d-7b22-a0d1-1d4ed0ed596f?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=1EHD&amp;paint=P0C36&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05DN,S06NX,S02BQ,S08WC,S03AC,S0775,S0676,S0710,S0534,S0337,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S06PA,S05AU,S06VB,S02PA,S0302,S04LN,S08TR,S0248,S0403,S0548,S03FA,S0760,S05DA,S07LG,S0420,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>44976</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B4" t="n">
-        <v>44976</v>
       </c>
       <c r="C4" t="n">
         <v>55900</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>55 900,00 €</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4" t="n">
         <v>22889</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>22889 km</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2025-03-01</t>
-        </is>
+      <c r="E4" s="2" t="n">
+        <v>45717</v>
+      </c>
+      <c r="F4" t="n">
+        <v>250</v>
+      </c>
+      <c r="G4" t="n">
+        <v>340</v>
       </c>
       <c r="H4" t="inlineStr">
-        <is>
-          <t>mars 2025</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>250</v>
-      </c>
-      <c r="J4" t="n">
-        <v>340</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -825,59 +844,70 @@
 }</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0194b79a-6463-7a38-8ef9-60a42d15a197?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0300&amp;fabric=FMANL&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05YA,S05DN,S06NX,S02BQ,S08WC,S03AC,S0710,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S06VB,S0302,S0544,S0548,S05DA,S07LG,S0420,S03FX,S04MC,S0491,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AS,S09QY,S02PA,S0688,S0403,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0194b79a-6463-7a38-8ef9-60a42d15a197?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0300&amp;fabric=FMANL&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05YA,S05DN,S06NX,S02BQ,S08WC,S03AC,S0710,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S06VB,S0302,S0544,S0548,S05DA,S07LG,S0420,S03FX,S04MC,S0491,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AS,S09QY,S02PA,S0688,S0403,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>44516</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>BMW i4 xDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B5" t="n">
-        <v>44516</v>
       </c>
       <c r="C5" t="n">
         <v>56900</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>56 900,00 €</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
+      <c r="D5" t="n">
         <v>21346</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>21346 km</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2025-02-01</t>
-        </is>
+      <c r="E5" s="2" t="n">
+        <v>45689</v>
+      </c>
+      <c r="F5" t="n">
+        <v>295</v>
+      </c>
+      <c r="G5" t="n">
+        <v>401</v>
       </c>
       <c r="H5" t="inlineStr">
-        <is>
-          <t>février 2025</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>295</v>
-      </c>
-      <c r="J5" t="n">
-        <v>401</v>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>295 kW (401 PS)</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -939,59 +969,70 @@
 }</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01927132-31bf-75f7-af77-3773e567d1e5?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41HD&amp;paint=P0C3Z&amp;fabric=FMAOI&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05YA,S05DN,S06NX,S02BQ,S03AC,S0676,S0710,S05AC,S0715,S04H0,S08WN,S0430,S0431,S04T2,S0552,S04T3,S02VL,S06VB,S02VF,S03GX,S0302,S0548,S05DA,S07LG,S0420,S04A2,S0491,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S04UR,S06PA,S05AU,S02PA,S08TR,S0248,S0403,S04HA,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01927132-31bf-75f7-af77-3773e567d1e5?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41HD&amp;paint=P0C3Z&amp;fabric=FMAOI&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05YA,S05DN,S06NX,S02BQ,S03AC,S0676,S0710,S05AC,S0715,S04H0,S08WN,S0430,S0431,S04T2,S0552,S04T3,S02VL,S06VB,S02VF,S03GX,S0302,S0548,S05DA,S07LG,S0420,S04A2,S0491,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S04UR,S06PA,S05AU,S02PA,S08TR,S0248,S0403,S04HA,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>39484</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>BMW i4 xDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B6" t="n">
-        <v>39484</v>
       </c>
       <c r="C6" t="n">
         <v>56900</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>56 900,00 €</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
+      <c r="D6" t="n">
         <v>24235</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>24235 km</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2025-01-01</t>
-        </is>
+      <c r="E6" s="2" t="n">
+        <v>45658</v>
+      </c>
+      <c r="F6" t="n">
+        <v>295</v>
+      </c>
+      <c r="G6" t="n">
+        <v>401</v>
       </c>
       <c r="H6" t="inlineStr">
-        <is>
-          <t>janvier 2025</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>295</v>
-      </c>
-      <c r="J6" t="n">
-        <v>401</v>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>295 kW (401 PS)</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -1050,59 +1091,70 @@
 }</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01924866-71fb-7076-894c-f956fe80f25a?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41HD&amp;paint=P0C4P&amp;fabric=FEPMI&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05YA,S05DN,S06NX,S02BQ,S03AC,S0676,S0710,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S02VL,S06VB,S02VF,S0302,S0548,S05DA,S07LG,S0420,S0491,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AU,S02PA,S04LN,S08TR,S0403,S03FA,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01924866-71fb-7076-894c-f956fe80f25a?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41HD&amp;paint=P0C4P&amp;fabric=FEPMI&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05YA,S05DN,S06NX,S02BQ,S03AC,S0676,S0710,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S02VL,S06VB,S02VF,S0302,S0548,S05DA,S07LG,S0420,S0491,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AU,S02PA,S04LN,S08TR,S0403,S03FA,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>27433</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>BMW i4 eDrive35 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B7" t="n">
-        <v>27433</v>
       </c>
       <c r="C7" t="n">
         <v>54900</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>54 900,00 €</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
+      <c r="D7" t="n">
         <v>5500</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>5500 km</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>2025-01-01</t>
-        </is>
+      <c r="E7" s="2" t="n">
+        <v>45658</v>
+      </c>
+      <c r="F7" t="n">
+        <v>210</v>
+      </c>
+      <c r="G7" t="n">
+        <v>286</v>
       </c>
       <c r="H7" t="inlineStr">
-        <is>
-          <t>janvier 2025</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>210</v>
-      </c>
-      <c r="J7" t="n">
-        <v>286</v>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>210 kW (286 PS)</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -1159,59 +1211,70 @@
 }</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0191ff1e-b3ad-7f85-9154-817a3faa61ed?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=11HD&amp;paint=P0C4P&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S06NX,S07M9,S08WC,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S06VB,S033B,S0302,S0544,S03M2,S0548,S05DA,S07LG,S0420,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S0494,S04UR,S06PA,S05AS,S04GQ,S09QY,S02PA,S04LN,S0688,S0403,S03FA,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0191ff1e-b3ad-7f85-9154-817a3faa61ed?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=11HD&amp;paint=P0C4P&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S06NX,S07M9,S08WC,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S06VB,S033B,S0302,S0544,S03M2,S0548,S05DA,S07LG,S0420,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S0494,S04UR,S06PA,S05AS,S04GQ,S09QY,S02PA,S04LN,S0688,S0403,S03FA,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N7" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>94567</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B8" t="n">
-        <v>94567</v>
       </c>
       <c r="C8" t="n">
         <v>57430</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>57 430,00 €</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
+      <c r="D8" t="n">
         <v>6279</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>6279 km</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2025-02-01</t>
-        </is>
+      <c r="E8" s="2" t="n">
+        <v>45689</v>
+      </c>
+      <c r="F8" t="n">
+        <v>250</v>
+      </c>
+      <c r="G8" t="n">
+        <v>340</v>
       </c>
       <c r="H8" t="inlineStr">
-        <is>
-          <t>février 2025</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>250</v>
-      </c>
-      <c r="J8" t="n">
-        <v>340</v>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -1266,59 +1329,70 @@
 }</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0191ff12-eb36-73d8-9dc2-7929d9c2c8fd?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C68&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S07M9,S08WC,S0775,S0676,S0710,S0754,S0534,S0337,S05AC,S0459,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S0552,S06PA,S05AS,S04GQ,S06VB,S033B,S02PA,S03GX,S0302,S04LN,S0248,S05DF,S0403,S03M2,S0548,S0760,S05DA,S0420,S06U3</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0191ff12-eb36-73d8-9dc2-7929d9c2c8fd?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C68&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S07M9,S08WC,S0775,S0676,S0710,S0754,S0534,S0337,S05AC,S0459,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S0552,S06PA,S05AS,S04GQ,S06VB,S033B,S02PA,S03GX,S0302,S04LN,S0248,S05DF,S0403,S03M2,S0548,S0760,S05DA,S0420,S06U3</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="n">
+        <v>27644</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B9" t="n">
-        <v>27644</v>
       </c>
       <c r="C9" t="n">
         <v>57900</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>57 900,00 €</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
+      <c r="D9" t="n">
         <v>4091</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>4091 km</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2025-02-01</t>
-        </is>
+      <c r="E9" s="2" t="n">
+        <v>45689</v>
+      </c>
+      <c r="F9" t="n">
+        <v>250</v>
+      </c>
+      <c r="G9" t="n">
+        <v>340</v>
       </c>
       <c r="H9" t="inlineStr">
-        <is>
-          <t>février 2025</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>250</v>
-      </c>
-      <c r="J9" t="n">
-        <v>340</v>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -1373,59 +1447,70 @@
 }</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0196cef0-4e7c-764b-8df8-ea95bdd9dd31?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C68&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S07M9,S08WC,S0775,S0676,S0710,S0754,S0534,S0337,S05AC,S0459,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S0552,S06PA,S05AS,S04GQ,S06VB,S033B,S02PA,S0302,S04LN,S0248,S05DF,S0403,S03FK,S03M2,S0548,S0760,S05DA,S0420,S06U3</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0196cef0-4e7c-764b-8df8-ea95bdd9dd31?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C68&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S07M9,S08WC,S0775,S0676,S0710,S0754,S0534,S0337,S05AC,S0459,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S0552,S06PA,S05AS,S04GQ,S06VB,S033B,S02PA,S0302,S04LN,S0248,S05DF,S0403,S03FK,S03M2,S0548,S0760,S05DA,S0420,S06U3</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="n">
+        <v>1806</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1806</v>
       </c>
       <c r="C10" t="n">
         <v>59900</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>59 900,00 €</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
+      <c r="D10" t="n">
         <v>6866</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>6866 km</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2025-02-01</t>
-        </is>
+      <c r="E10" s="2" t="n">
+        <v>45689</v>
+      </c>
+      <c r="F10" t="n">
+        <v>250</v>
+      </c>
+      <c r="G10" t="n">
+        <v>340</v>
       </c>
       <c r="H10" t="inlineStr">
-        <is>
-          <t>février 2025</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>250</v>
-      </c>
-      <c r="J10" t="n">
-        <v>340</v>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -1482,59 +1567,70 @@
 }</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01919331-2be9-7cf9-af6a-2b42dfa0a180?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C4P&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S07M9,S08WC,S03AC,S0775,S0676,S0710,S0754,S0534,S0337,S05AC,S0459,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S0552,S06PA,S05AS,S04GQ,S06VB,S033B,S02PA,S0302,S04LN,S0248,S05DF,S0403,S03FK,S03M2,S0548,S0760,S05DA,S0420,S06U3</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01919331-2be9-7cf9-af6a-2b42dfa0a180?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C4P&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S07M9,S08WC,S03AC,S0775,S0676,S0710,S0754,S0534,S0337,S05AC,S0459,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S0552,S06PA,S05AS,S04GQ,S06VB,S033B,S02PA,S0302,S04LN,S0248,S05DF,S0403,S03FK,S03M2,S0548,S0760,S05DA,S0420,S06U3</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N10" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="n">
+        <v>42538</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B11" t="n">
-        <v>42538</v>
       </c>
       <c r="C11" t="n">
         <v>56900</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>56 900,00 €</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
+      <c r="D11" t="n">
         <v>5735</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>5735 km</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2025-01-01</t>
-        </is>
+      <c r="E11" s="2" t="n">
+        <v>45658</v>
+      </c>
+      <c r="F11" t="n">
+        <v>250</v>
+      </c>
+      <c r="G11" t="n">
+        <v>340</v>
       </c>
       <c r="H11" t="inlineStr">
-        <is>
-          <t>janvier 2025</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>250</v>
-      </c>
-      <c r="J11" t="n">
-        <v>340</v>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -1589,59 +1685,70 @@
 }</t>
         </is>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0190025a-3cf8-7ea6-bb76-f50ac9e66849?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0X1E&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S03MF,S05DM,S06NX,S06WC,S07M9,S08WC,S0710,S0754,S05AC,S0715,S08WN,S0430,S08SM,S0431,S04T2,S0552,S06VB,S033B,S0302,S0544,S03M2,S0548,S05DA,S07LG,S0420,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S0494,S04UR,S06PA,S04GQ,S09QY,S02PA,S04LN,S0403,S03FK,S0760,S06U2,S0322,S0488</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0190025a-3cf8-7ea6-bb76-f50ac9e66849?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0X1E&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S03MF,S05DM,S06NX,S06WC,S07M9,S08WC,S0710,S0754,S05AC,S0715,S08WN,S0430,S08SM,S0431,S04T2,S0552,S06VB,S033B,S0302,S0544,S03M2,S0548,S05DA,S07LG,S0420,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S0494,S04UR,S06PA,S04GQ,S09QY,S02PA,S04LN,S0403,S03FK,S0760,S06U2,S0322,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="n">
+        <v>45201</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B12" t="n">
-        <v>45201</v>
       </c>
       <c r="C12" t="n">
         <v>56750</v>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>56 750,00 €</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
+      <c r="D12" t="n">
         <v>21998</v>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>21998 km</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2024-12-01</t>
-        </is>
+      <c r="E12" s="2" t="n">
+        <v>45627</v>
+      </c>
+      <c r="F12" t="n">
+        <v>250</v>
+      </c>
+      <c r="G12" t="n">
+        <v>340</v>
       </c>
       <c r="H12" t="inlineStr">
-        <is>
-          <t>décembre 2024</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>250</v>
-      </c>
-      <c r="J12" t="n">
-        <v>340</v>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -1700,59 +1807,70 @@
 }</t>
         </is>
       </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01908a6c-f5bd-7114-8611-2ea29b6a60a0?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C5Y&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05YA,S05DN,S06NX,S07M9,S08WC,S0676,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S06VB,S033B,S0302,S03M2,S0548,S05DA,S07LG,S0420,S03FX,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AU,S04GQ,S02PA,S04LN,S08TR,S0403,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01908a6c-f5bd-7114-8611-2ea29b6a60a0?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C5Y&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05YA,S05DN,S06NX,S07M9,S08WC,S0676,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S06VB,S033B,S0302,S03M2,S0548,S05DA,S07LG,S0420,S03FX,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AU,S04GQ,S02PA,S04LN,S08TR,S0403,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" t="n">
+        <v>93924</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B13" t="n">
-        <v>93924</v>
       </c>
       <c r="C13" t="n">
         <v>58390</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>58 390,00 €</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
+      <c r="D13" t="n">
         <v>10095</v>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>10095 km</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2025-01-01</t>
-        </is>
+      <c r="E13" s="2" t="n">
+        <v>45658</v>
+      </c>
+      <c r="F13" t="n">
+        <v>250</v>
+      </c>
+      <c r="G13" t="n">
+        <v>340</v>
       </c>
       <c r="H13" t="inlineStr">
-        <is>
-          <t>janvier 2025</t>
-        </is>
-      </c>
-      <c r="I13" t="n">
-        <v>250</v>
-      </c>
-      <c r="J13" t="n">
-        <v>340</v>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -1809,59 +1927,70 @@
 }</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01905f02-b6f6-7048-b969-7866a99e3a1e?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0475&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S06NX,S07M9,S08WC,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S06VB,S033B,S0302,S05DF,S03M2,S0548,S05DA,S07LG,S0420,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S0494,S04UR,S06PA,S05AS,S04GQ,S02PA,S04LN,S0688,S0403,S03FK,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/01905f02-b6f6-7048-b969-7866a99e3a1e?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0475&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S06NX,S07M9,S08WC,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S06VB,S033B,S0302,S05DF,S03M2,S0548,S05DA,S07LG,S0420,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S0494,S04UR,S06PA,S05AS,S04GQ,S02PA,S04LN,S0688,S0403,S03FK,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N13" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" t="n">
+        <v>39694</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B14" t="n">
-        <v>39694</v>
       </c>
       <c r="C14" t="n">
         <v>53900</v>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>53 900,00 €</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
+      <c r="D14" t="n">
         <v>19539</v>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>19539 km</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
+      <c r="E14" s="2" t="n">
+        <v>45566</v>
+      </c>
+      <c r="F14" t="n">
+        <v>250</v>
+      </c>
+      <c r="G14" t="n">
+        <v>340</v>
       </c>
       <c r="H14" t="inlineStr">
-        <is>
-          <t>octobre 2024</t>
-        </is>
-      </c>
-      <c r="I14" t="n">
-        <v>250</v>
-      </c>
-      <c r="J14" t="n">
-        <v>340</v>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
         <is>
           <t>{
   "ConnectedDrive FA": [
@@ -1920,59 +2049,70 @@
 }</t>
         </is>
       </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0191c219-3f0f-7927-8560-b2f4464f3d69?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C36&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S04NW,S05YA,S05DN,S06NX,S02BQ,S08WC,S0775,S0676,S0710,S0534,S0337,S05AC,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S04V1,S0494,S0430,S04UR,S0431,S04T2,S0552,S04T3,S06PA,S05AU,S06VB,S02PA,S0302,S04LN,S08TR,S0403,S03FK,S0548,S0760,S05DA,S07LG,S0420,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/0191c219-3f0f-7927-8560-b2f4464f3d69?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C36&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S04NW,S05YA,S05DN,S06NX,S02BQ,S08WC,S0775,S0676,S0710,S0534,S0337,S05AC,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S04V1,S0494,S0430,S04UR,S0431,S04T2,S0552,S04T3,S06PA,S05AU,S06VB,S02PA,S0302,S04LN,S08TR,S0403,S03FK,S0548,S0760,S05DA,S07LG,S0420,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N14" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" t="n">
+        <v>44606</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B15" t="n">
-        <v>44606</v>
       </c>
       <c r="C15" t="n">
         <v>56900</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>56 900,00 €</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
+      <c r="D15" t="n">
         <v>8202</v>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>8202 km</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2024-08-01</t>
-        </is>
+      <c r="E15" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="F15" t="n">
+        <v>250</v>
+      </c>
+      <c r="G15" t="n">
+        <v>340</v>
       </c>
       <c r="H15" t="inlineStr">
-        <is>
-          <t>août 2024</t>
-        </is>
-      </c>
-      <c r="I15" t="n">
-        <v>250</v>
-      </c>
-      <c r="J15" t="n">
-        <v>340</v>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
         <is>
           <t>{
   "ConnectedDrive FA": [
@@ -2042,59 +2182,70 @@
 }</t>
         </is>
       </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e956b-fc6f-7af8-bad5-52a5bd11a952?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C5Y&amp;fabric=FMANL&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05YA,S05DN,S06NX,S07M9,S0676,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S06VB,S033B,S0302,S0544,S03M2,S0548,S05DA,S07LG,S0420,S03FX,S04MC,S0491,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AS,S04GQ,S09QY,S02PA,S0403,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e956b-fc6f-7af8-bad5-52a5bd11a952?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C5Y&amp;fabric=FMANL&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05YA,S05DN,S06NX,S07M9,S0676,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S06VB,S033B,S0302,S0544,S03M2,S0548,S05DA,S07LG,S0420,S03FX,S04MC,S0491,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AS,S04GQ,S09QY,S02PA,S0403,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N15" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" t="n">
+        <v>27566</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B16" t="n">
-        <v>27566</v>
       </c>
       <c r="C16" t="n">
         <v>58900</v>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>58 900,00 €</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
+      <c r="D16" t="n">
         <v>17518</v>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>17518 km</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2024-08-01</t>
-        </is>
+      <c r="E16" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="F16" t="n">
+        <v>250</v>
+      </c>
+      <c r="G16" t="n">
+        <v>340</v>
       </c>
       <c r="H16" t="inlineStr">
-        <is>
-          <t>août 2024</t>
-        </is>
-      </c>
-      <c r="I16" t="n">
-        <v>250</v>
-      </c>
-      <c r="J16" t="n">
-        <v>340</v>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
         <is>
           <t>{
   "ConnectedDrive FA": [
@@ -2163,59 +2314,70 @@
 }</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e9600-c9a6-7eee-b980-3a372a959b5d?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C36&amp;fabric=FEPMI&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05YA,S05DN,S06NX,S07M9,S0676,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S06VB,S033B,S0302,S0544,S03M2,S0548,S05DA,S07LG,S0420,S0491,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AS,S04GQ,S09QY,S02PA,S04LN,S0403,S03FK,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e9600-c9a6-7eee-b980-3a372a959b5d?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0C36&amp;fabric=FEPMI&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05YA,S05DN,S06NX,S07M9,S0676,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S06VB,S033B,S0302,S0544,S03M2,S0548,S05DA,S07LG,S0420,S0491,S0775,S0534,S0337,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AS,S04GQ,S09QY,S02PA,S04LN,S0403,S03FK,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N16" t="b">
+        <v>1</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" t="n">
+        <v>43611</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B17" t="n">
-        <v>43611</v>
       </c>
       <c r="C17" t="n">
         <v>54750</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>54 750,00 €</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
+      <c r="D17" t="n">
         <v>25489</v>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>25489 km</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>2024-08-01</t>
-        </is>
+      <c r="E17" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="F17" t="n">
+        <v>250</v>
+      </c>
+      <c r="G17" t="n">
+        <v>340</v>
       </c>
       <c r="H17" t="inlineStr">
-        <is>
-          <t>août 2024</t>
-        </is>
-      </c>
-      <c r="I17" t="n">
-        <v>250</v>
-      </c>
-      <c r="J17" t="n">
-        <v>340</v>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
         <is>
           <t>{
   "ConnectedDrive FA": [
@@ -2285,59 +2447,70 @@
 }</t>
         </is>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e9600-d868-7e02-90ac-261639db895c?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0300&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05YA,S05DN,S06NX,S02BQ,S03AC,S0710,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S02VL,S06VB,S02VF,S0302,S0548,S05DA,S07LG,S0420,S03FX,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AU,S02PA,S04LN,S08TR,S0688,S0248,S0403,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e9600-d868-7e02-90ac-261639db895c?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0300&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05YA,S05DN,S06NX,S02BQ,S03AC,S0710,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S04T3,S02VL,S06VB,S02VF,S0302,S0548,S05DA,S07LG,S0420,S03FX,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AU,S02PA,S04LN,S08TR,S0688,S0248,S0403,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" t="n">
+        <v>27404</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>BMW i4 xDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B18" t="n">
-        <v>27404</v>
       </c>
       <c r="C18" t="n">
         <v>59900</v>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>59 900,00 €</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
+      <c r="D18" t="n">
         <v>10254</v>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>10254 km</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>2024-08-01</t>
-        </is>
+      <c r="E18" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="F18" t="n">
+        <v>295</v>
+      </c>
+      <c r="G18" t="n">
+        <v>401</v>
       </c>
       <c r="H18" t="inlineStr">
-        <is>
-          <t>août 2024</t>
-        </is>
-      </c>
-      <c r="I18" t="n">
-        <v>295</v>
-      </c>
-      <c r="J18" t="n">
-        <v>401</v>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>295 kW (401 PS)</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -2391,59 +2564,70 @@
 }</t>
         </is>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/019059b1-bd37-7c22-8d90-dd4f218b8828?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41HD&amp;paint=P0C4P&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05DN,S06NX,S02BQ,S0775,S0676,S0710,S0534,S0337,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S06PA,S05AS,S02VL,S06VB,S02VF,S02PA,S0302,S04LN,S0248,S05DF,S0403,S03FK,S0548,S0760,S05DA,S07LG,S0420,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/019059b1-bd37-7c22-8d90-dd4f218b8828?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41HD&amp;paint=P0C4P&amp;fabric=FKHSW&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S05DN,S06NX,S02BQ,S0775,S0676,S0710,S0534,S0337,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S04UR,S0431,S04T2,S06PA,S05AS,S02VL,S06VB,S02VF,S02PA,S0302,S04LN,S0248,S05DF,S0403,S03FK,S0548,S0760,S05DA,S07LG,S0420,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N18" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" t="n">
+        <v>20301</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B19" t="n">
-        <v>20301</v>
       </c>
       <c r="C19" t="n">
         <v>54995</v>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>54 995,00 €</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
+      <c r="D19" t="n">
         <v>22375</v>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>22375 km</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
+      <c r="E19" s="2" t="n">
+        <v>45566</v>
+      </c>
+      <c r="F19" t="n">
+        <v>250</v>
+      </c>
+      <c r="G19" t="n">
+        <v>340</v>
       </c>
       <c r="H19" t="inlineStr">
-        <is>
-          <t>octobre 2024</t>
-        </is>
-      </c>
-      <c r="I19" t="n">
-        <v>250</v>
-      </c>
-      <c r="J19" t="n">
-        <v>340</v>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -2507,59 +2691,70 @@
 }</t>
         </is>
       </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e94f5-4f5c-790e-9a77-87c396b972e0?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0475&amp;fabric=FVATQ&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S04NW,S05DN,S06NX,S07M9,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S02VL,S06VB,S033B,S02VF,S03GX,S0302,S03M2,S0548,S05DA,S07LG,S0420,S04A2,S0491,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AU,S04H1,S04GQ,S02PA,S08TR,S0688,S0248,S0403,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e94f5-4f5c-790e-9a77-87c396b972e0?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=21HD&amp;paint=P0475&amp;fabric=FVATQ&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S04NW,S05DN,S06NX,S07M9,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S02VL,S06VB,S033B,S02VF,S03GX,S0302,S03M2,S0548,S05DA,S07LG,S0420,S04A2,S0491,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S06PA,S05AU,S04H1,S04GQ,S02PA,S08TR,S0688,S0248,S0403,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" t="n">
+        <v>40022</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>BMW i4 xDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B20" t="n">
-        <v>40022</v>
       </c>
       <c r="C20" t="n">
         <v>53900</v>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>53 900,00 €</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
+      <c r="D20" t="n">
         <v>35183</v>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>35183 km</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>2024-08-01</t>
-        </is>
+      <c r="E20" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="F20" t="n">
+        <v>295</v>
+      </c>
+      <c r="G20" t="n">
+        <v>401</v>
       </c>
       <c r="H20" t="inlineStr">
-        <is>
-          <t>août 2024</t>
-        </is>
-      </c>
-      <c r="I20" t="n">
-        <v>295</v>
-      </c>
-      <c r="J20" t="n">
-        <v>401</v>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>295 kW (401 PS)</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -2619,59 +2814,70 @@
 }</t>
         </is>
       </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018fa5f6-947f-71ba-81da-17d4dc327cd6?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41HD&amp;paint=P0C3Z&amp;fabric=FVATQ&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S06NX,S07M9,S03AC,S0676,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S02VL,S06VB,S033B,S02VF,S0302,S03M2,S0548,S05DA,S07LG,S0420,S0491,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S0494,S04UR,S06PA,S05AU,S04GQ,S02PA,S04LN,S08TR,S0403,S03FK,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018fa5f6-947f-71ba-81da-17d4dc327cd6?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41HD&amp;paint=P0C3Z&amp;fabric=FVATQ&amp;modelRangeCode=G26&amp;options=S08WD,S07A2,S03MF,S05DN,S06NX,S07M9,S03AC,S0676,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S0552,S02VL,S06VB,S033B,S02VF,S0302,S03M2,S0548,S05DA,S07LG,S0420,S0491,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S0494,S04UR,S06PA,S05AU,S04GQ,S02PA,S04LN,S08TR,S0403,S03FK,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" t="n">
+        <v>27838</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B21" t="n">
-        <v>27838</v>
       </c>
       <c r="C21" t="n">
         <v>54700</v>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>54 700,00 €</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
+      <c r="D21" t="n">
         <v>29650</v>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>29650 km</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>2024-04-01</t>
-        </is>
+      <c r="E21" s="2" t="n">
+        <v>45383</v>
+      </c>
+      <c r="F21" t="n">
+        <v>250</v>
+      </c>
+      <c r="G21" t="n">
+        <v>340</v>
       </c>
       <c r="H21" t="inlineStr">
-        <is>
-          <t>avril 2024</t>
-        </is>
-      </c>
-      <c r="I21" t="n">
-        <v>250</v>
-      </c>
-      <c r="J21" t="n">
-        <v>340</v>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -2730,59 +2936,70 @@
 }</t>
         </is>
       </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e94dc-a63e-75a9-99ba-3d727aedd0f0?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=71AW&amp;paint=P0A96&amp;fabric=FMAH7&amp;modelRangeCode=G26&amp;options=S08WD,S0ZB1,S0ZEV,S03MF,S05DM,S06NX,S07M9,S03AC,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S04AW,S06VB,S033B,S0302,S0548,S05DA,S0420,S04MC,S0491,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S0494,S04UR,S05AU,S04GQ,S02PA,S08TR,S0688,S0248,S0ZT1,S0403,S03FK,S05AZ,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e94dc-a63e-75a9-99ba-3d727aedd0f0?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=71AW&amp;paint=P0A96&amp;fabric=FMAH7&amp;modelRangeCode=G26&amp;options=S08WD,S0ZB1,S0ZEV,S03MF,S05DM,S06NX,S07M9,S03AC,S0710,S0754,S05AC,S0715,S08WN,S0430,S0431,S04T2,S04AW,S06VB,S033B,S0302,S0548,S05DA,S0420,S04MC,S0491,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S0494,S04UR,S05AU,S04GQ,S02PA,S08TR,S0688,S0248,S0ZT1,S0403,S03FK,S05AZ,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N21" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" t="n">
+        <v>28441</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B22" t="n">
-        <v>28441</v>
       </c>
       <c r="C22" t="n">
         <v>56700</v>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>56 700,00 €</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
+      <c r="D22" t="n">
         <v>22969</v>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>22969 km</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2024-07-01</t>
-        </is>
+      <c r="E22" s="2" t="n">
+        <v>45474</v>
+      </c>
+      <c r="F22" t="n">
+        <v>250</v>
+      </c>
+      <c r="G22" t="n">
+        <v>340</v>
       </c>
       <c r="H22" t="inlineStr">
-        <is>
-          <t>juillet 2024</t>
-        </is>
-      </c>
-      <c r="I22" t="n">
-        <v>250</v>
-      </c>
-      <c r="J22" t="n">
-        <v>340</v>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -2842,59 +3059,70 @@
 }</t>
         </is>
       </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e94b9-7a93-78c6-9a35-ed47a7f9b187?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=71AW&amp;paint=P0A96&amp;fabric=FMANL&amp;modelRangeCode=G26&amp;options=S08WD,S0ZB1,S0ZEV,S03MF,S05DN,S06NX,S07M9,S03AC,S0710,S0754,S0711,S05AC,S0715,S08WN,S0430,S0431,S04T2,S04AW,S06VB,S033B,S0302,S03M2,S0548,S05DA,S0420,S04MC,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S05AU,S04GQ,S02PA,S08TR,S0688,S0ZT1,S0403,S03FK,S05AZ,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e94b9-7a93-78c6-9a35-ed47a7f9b187?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=71AW&amp;paint=P0A96&amp;fabric=FMANL&amp;modelRangeCode=G26&amp;options=S08WD,S0ZB1,S0ZEV,S03MF,S05DN,S06NX,S07M9,S03AC,S0710,S0754,S0711,S05AC,S0715,S08WN,S0430,S0431,S04T2,S04AW,S06VB,S033B,S0302,S03M2,S0548,S05DA,S0420,S04MC,S0775,S0534,S0337,S0459,S08R3,S06AE,S06AF,S0493,S04V1,S0494,S04UR,S05AU,S04GQ,S02PA,S08TR,S0688,S0ZT1,S0403,S03FK,S05AZ,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" t="n">
+        <v>9811</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B23" t="n">
-        <v>9811</v>
       </c>
       <c r="C23" t="n">
         <v>52850</v>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>52 850,00 €</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
+      <c r="D23" t="n">
         <v>9343</v>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>9343 km</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2024-04-01</t>
-        </is>
+      <c r="E23" s="2" t="n">
+        <v>45383</v>
+      </c>
+      <c r="F23" t="n">
+        <v>250</v>
+      </c>
+      <c r="G23" t="n">
+        <v>340</v>
       </c>
       <c r="H23" t="inlineStr">
-        <is>
-          <t>avril 2024</t>
-        </is>
-      </c>
-      <c r="I23" t="n">
-        <v>250</v>
-      </c>
-      <c r="J23" t="n">
-        <v>340</v>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -2950,59 +3178,70 @@
 }</t>
         </is>
       </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e955b-3d80-7d13-8e2f-9b7f48918c7c?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=71AW&amp;paint=P0C4E&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S08WD,S05DN,S06NX,S0775,S0676,S0710,S0534,S0337,S05AC,S0459,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S04V1,S0494,S0430,S04UR,S0431,S04T2,S04T3,S06PA,S05AS,S02VL,S04AW,S09QY,S06VB,S02VF,S02PA,S0302,S0544,S0403,S0548,S03FA,S0760,S05DA,S0420,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e955b-3d80-7d13-8e2f-9b7f48918c7c?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=71AW&amp;paint=P0C4E&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S08WD,S05DN,S06NX,S0775,S0676,S0710,S0534,S0337,S05AC,S0459,S08R3,S06AE,S0715,S06AF,S0493,S08WN,S04V1,S0494,S0430,S04UR,S0431,S04T2,S04T3,S06PA,S05AS,S02VL,S04AW,S09QY,S06VB,S02VF,S02PA,S0302,S0544,S0403,S0548,S03FA,S0760,S05DA,S0420,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N23" t="b">
+        <v>1</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" t="n">
+        <v>88830</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B24" t="n">
-        <v>88830</v>
       </c>
       <c r="C24" t="n">
         <v>54999</v>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>54 999,00 €</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
+      <c r="D24" t="n">
         <v>19325</v>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>19325 km</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>2024-03-01</t>
-        </is>
+      <c r="E24" s="2" t="n">
+        <v>45352</v>
+      </c>
+      <c r="F24" t="n">
+        <v>250</v>
+      </c>
+      <c r="G24" t="n">
+        <v>340</v>
       </c>
       <c r="H24" t="inlineStr">
-        <is>
-          <t>mars 2024</t>
-        </is>
-      </c>
-      <c r="I24" t="n">
-        <v>250</v>
-      </c>
-      <c r="J24" t="n">
-        <v>340</v>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -3058,59 +3297,70 @@
 }</t>
         </is>
       </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e956d-853b-7342-badd-9e8d9e6655f6?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=71AW&amp;paint=P0C31&amp;fabric=FVAEW&amp;modelRangeCode=G26&amp;options=S03FX,S0491,S05DN,S06NX,S08WT,S0775,S0710,S0534,S0337,S05AC,S0459,S06AE,S0715,S06AF,S0493,S08WN,S04V1,S0494,S0430,S04UR,S0431,S04T2,S04T3,S06PA,S02VL,S05AU,S04AW,S06VB,S02VF,S02PA,S0302,S08TR,S0688,S0403,S0548,S05AZ,S0760,S05DA,S0420,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e956d-853b-7342-badd-9e8d9e6655f6?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=71AW&amp;paint=P0C31&amp;fabric=FVAEW&amp;modelRangeCode=G26&amp;options=S03FX,S0491,S05DN,S06NX,S08WT,S0775,S0710,S0534,S0337,S05AC,S0459,S06AE,S0715,S06AF,S0493,S08WN,S04V1,S0494,S0430,S04UR,S0431,S04T2,S04T3,S06PA,S02VL,S05AU,S04AW,S06VB,S02VF,S02PA,S0302,S08TR,S0688,S0403,S0548,S05AZ,S0760,S05DA,S0420,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" t="n">
+        <v>1746</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B25" t="n">
-        <v>1746</v>
       </c>
       <c r="C25" t="n">
         <v>53900</v>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>53 900,00 €</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
+      <c r="D25" t="n">
         <v>19860</v>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>19860 km</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>2024-08-01</t>
-        </is>
+      <c r="E25" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="F25" t="n">
+        <v>250</v>
+      </c>
+      <c r="G25" t="n">
+        <v>340</v>
       </c>
       <c r="H25" t="inlineStr">
-        <is>
-          <t>août 2024</t>
-        </is>
-      </c>
-      <c r="I25" t="n">
-        <v>250</v>
-      </c>
-      <c r="J25" t="n">
-        <v>340</v>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -3167,59 +3417,70 @@
 }</t>
         </is>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e91f0-d524-70a8-89c5-852fec977271?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=71AW&amp;paint=P0C3Z&amp;fabric=FMANL&amp;modelRangeCode=G26&amp;options=S0ZB1,S0ZEV,S03MF,S05DN,S06NX,S07M9,S08WT,S0710,S0754,S0715,S08WN,S0430,S0431,S04T2,S04AW,S06VB,S033B,S0302,S03M2,S0548,S05DA,S0420,S0491,S0775,S0534,S0337,S0459,S06AE,S06AF,S0493,S0494,S04UR,S0ZLD,S05AU,S04GQ,S02PA,S04LN,S08TR,S0688,S0248,S0ZT1,S0403,S03FK,S0760,S0322,S06U3,S0488</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e91f0-d524-70a8-89c5-852fec977271?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=71AW&amp;paint=P0C3Z&amp;fabric=FMANL&amp;modelRangeCode=G26&amp;options=S0ZB1,S0ZEV,S03MF,S05DN,S06NX,S07M9,S08WT,S0710,S0754,S0715,S08WN,S0430,S0431,S04T2,S04AW,S06VB,S033B,S0302,S03M2,S0548,S05DA,S0420,S0491,S0775,S0534,S0337,S0459,S06AE,S06AF,S0493,S0494,S04UR,S0ZLD,S05AU,S04GQ,S02PA,S04LN,S08TR,S0688,S0248,S0ZT1,S0403,S03FK,S0760,S0322,S06U3,S0488</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N25" t="b">
+        <v>1</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" t="n">
+        <v>92901</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>BMW i4 eDrive35 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B26" t="n">
-        <v>92901</v>
       </c>
       <c r="C26" t="n">
         <v>48760</v>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>48 760,00 €</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
+      <c r="D26" t="n">
         <v>29630</v>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>29630 km</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>2024-04-01</t>
-        </is>
+      <c r="E26" s="2" t="n">
+        <v>45383</v>
+      </c>
+      <c r="F26" t="n">
+        <v>210</v>
+      </c>
+      <c r="G26" t="n">
+        <v>286</v>
       </c>
       <c r="H26" t="inlineStr">
-        <is>
-          <t>avril 2024</t>
-        </is>
-      </c>
-      <c r="I26" t="n">
-        <v>210</v>
-      </c>
-      <c r="J26" t="n">
-        <v>286</v>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>210 kW (286 PS)</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -3269,59 +3530,70 @@
 }</t>
         </is>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e94de-4570-7d07-89f7-f5279c8276cf?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41AW&amp;paint=P0475&amp;fabric=FMAH7&amp;modelRangeCode=G26&amp;options=S03MF,S0491,S0ZT7,S05DN,S07M9,S0775,S0676,S0710,S0754,S0534,S0337,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S0431,S04T2,S05AU,S0ZHX,S04GQ,S0ZS7,S06VB,S033B,S02PA,S0302,S04LN,S08TR,S0248,S0403,S03FK,S03M2,S0548,S0760,S05DA,S0420,S0ZUN,S0322,S06U3</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e94de-4570-7d07-89f7-f5279c8276cf?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=41AW&amp;paint=P0475&amp;fabric=FMAH7&amp;modelRangeCode=G26&amp;options=S03MF,S0491,S0ZT7,S05DN,S07M9,S0775,S0676,S0710,S0754,S0534,S0337,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S0431,S04T2,S05AU,S0ZHX,S04GQ,S0ZS7,S06VB,S033B,S02PA,S0302,S04LN,S08TR,S0248,S0403,S03FK,S03M2,S0548,S0760,S05DA,S0420,S0ZUN,S0322,S06U3</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" t="n">
+        <v>27864</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>BMW i4 eDrive40 Gran Coupé</t>
         </is>
-      </c>
-      <c r="B27" t="n">
-        <v>27864</v>
       </c>
       <c r="C27" t="n">
         <v>49950</v>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>49 950,00 €</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
+      <c r="D27" t="n">
         <v>14813</v>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>14813 km</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>2024-01-01</t>
-        </is>
+      <c r="E27" s="2" t="n">
+        <v>45292</v>
+      </c>
+      <c r="F27" t="n">
+        <v>250</v>
+      </c>
+      <c r="G27" t="n">
+        <v>340</v>
       </c>
       <c r="H27" t="inlineStr">
-        <is>
-          <t>janvier 2024</t>
-        </is>
-      </c>
-      <c r="I27" t="n">
-        <v>250</v>
-      </c>
-      <c r="J27" t="n">
-        <v>340</v>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>250 kW (340 PS)</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
         <is>
           <t>{
   "Charging": [
@@ -3369,9 +3641,42 @@
 }</t>
         </is>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e9336-94c6-7339-8322-38f58b792404?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=71AW&amp;paint=P0475&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S03FX,S03MF,S05DM,S06NX,S07M9,S08WT,S0775,S0710,S0754,S0534,S0337,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S0431,S04T2,S05AU,S04AW,S04GQ,S06VB,S033B,S02PA,S0302,S04LN,S08TR,S0403,S03M2,S0548,S0760,S05DA,S0420,S06U3</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>https://www.bmw.be/fr-be/sl/stocklocator_uc/details/018e9336-94c6-7339-8322-38f58b792404?filters=%257B%2522MARKETING_MODEL_RANGE%2522%253A%255B%2522i4_G26E%2522%252C%2522i5_G61E%2522%252C%2522i5_G60E%2522%255D%252C%2522PRICE%2522%253A%255Bnull%252C60000%255D%252C%2522REGISTRATION_YEAR%2522%253A%255B2024%252C-1%255D%252C%2522EQUIPMENT_GROUPS%2522%253A%257B%2522Default%2522%253A%255B%2522M%2520leather%2520steering%2520wheel%2522%252C%2522Sun%2520roof%2522%255D%252C%2522favorites%2522%253A%255B%2522M%2520Sport%2520package%2522%255D%257D%257D&amp;modelCode=71AW&amp;paint=P0475&amp;fabric=FKHKC&amp;modelRangeCode=G26&amp;options=S03FX,S03MF,S05DM,S06NX,S07M9,S08WT,S0775,S0710,S0754,S0534,S0337,S06AE,S0715,S06AF,S0493,S08WN,S0494,S0430,S0431,S04T2,S05AU,S04AW,S04GQ,S06VB,S033B,S02PA,S0302,S04LN,S08TR,S0403,S03M2,S0548,S0760,S05DA,S0420,S06U3</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
         </is>
       </c>
     </row>

</xml_diff>